<commit_message>
revising 1-5 handout, link to handout and homework
</commit_message>
<xml_diff>
--- a/handouts/chapter_1_5_handout.xlsx
+++ b/handouts/chapter_1_5_handout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RData\BYUI-Timeseries-Drafts\handouts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RussellStuff\Time series personal work\timeseries\handouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683AC7F6-8F81-4DA6-824A-9603C8C8FD49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7456007-9217-492C-A54C-2E211A1721FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB73943A-C465-40BE-817C-B9991112161C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{CB73943A-C465-40BE-817C-B9991112161C}"/>
   </bookViews>
   <sheets>
     <sheet name="Workbook" sheetId="2" r:id="rId1"/>
@@ -233,12 +233,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -430,15 +430,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color theme="1"/>
       </right>
@@ -516,19 +507,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -625,11 +603,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -668,8 +731,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -682,47 +743,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -745,17 +790,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2435,8 +2529,8 @@
       <xdr:rowOff>129413</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="196079" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2518,7 +2612,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2583,8 +2677,8 @@
       <xdr:rowOff>83693</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="252762" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -2678,7 +2772,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -2749,8 +2843,8 @@
       <xdr:rowOff>83693</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="180819" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2844,7 +2938,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2915,8 +3009,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="320040" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -3010,7 +3104,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -3075,8 +3169,8 @@
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="196079" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -3158,7 +3252,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -3537,28 +3631,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABFF2E6-1E13-48EF-9BE3-D6C90C46BEC8}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" customWidth="1"/>
+    <col min="14" max="14" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:4" ht="48.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="46"/>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -3568,7 +3662,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
@@ -3582,7 +3676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -3592,151 +3686,151 @@
       <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="51" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="8">
         <v>1.24</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="52">
         <v>1.3149999999999999</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="61" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="49">
         <v>1.71</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="61" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="8">
         <v>2.42</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="53">
         <v>1.829</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="61" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="49">
         <v>1.71</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="61" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="14">
         <v>1.71</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="55">
         <v>2.2509999999999999</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="62" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="50">
         <v>2.19</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="54">
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <v>4.37</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="56">
         <v>3.1360000000000001</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="15">
         <v>1.393</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <v>3.42</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <v>3.4689999999999999</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="15">
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <v>3.42</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <v>3.956</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="15">
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="14">
         <v>3.14</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <v>4.4740000000000002</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="15">
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
@@ -3750,7 +3844,7 @@
         <v>1.5249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -3764,7 +3858,7 @@
         <v>0.78500000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
@@ -3778,7 +3872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -3792,7 +3886,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -3806,7 +3900,7 @@
         <v>1.2190000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>21</v>
       </c>
@@ -3820,7 +3914,7 @@
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>22</v>
       </c>
@@ -3834,47 +3928,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="26">
         <v>89.498000000000005</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:5" ht="34.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>2005</v>
       </c>
@@ -3884,31 +3978,31 @@
       <c r="C27" t="s">
         <v>2</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>2006</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="20">
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>2007</v>
       </c>
@@ -3921,11 +4015,11 @@
       <c r="D29" s="1">
         <v>0.86399999999999999</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="20">
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="7">
         <v>2008</v>
       </c>
@@ -3938,11 +4032,11 @@
       <c r="D30" s="1">
         <v>0.68300000000000005</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="20">
         <v>1.325</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <v>2009</v>
       </c>
@@ -3955,11 +4049,11 @@
       <c r="D31" s="1">
         <v>0.83399999999999996</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="20">
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>2010</v>
       </c>
@@ -3972,11 +4066,11 @@
       <c r="D32" s="1">
         <v>0.84899999999999998</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="20">
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>2011</v>
       </c>
@@ -3993,7 +4087,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>2012</v>
       </c>
@@ -4006,11 +4100,11 @@
       <c r="D34">
         <v>0.86499999999999999</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="19">
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="7">
         <v>2013</v>
       </c>
@@ -4023,11 +4117,11 @@
       <c r="D35">
         <v>0.81899999999999995</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="19">
         <v>0.85599999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <v>2014</v>
       </c>
@@ -4040,11 +4134,11 @@
       <c r="D36">
         <v>0.78300000000000003</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="19">
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
         <v>2015</v>
       </c>
@@ -4057,11 +4151,11 @@
       <c r="D37">
         <v>0.84699999999999998</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="19">
         <v>0.89100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="7">
         <v>2016</v>
       </c>
@@ -4074,11 +4168,11 @@
       <c r="D38">
         <v>0.78100000000000003</v>
       </c>
-      <c r="E38" s="21">
+      <c r="E38" s="19">
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
         <v>2017</v>
       </c>
@@ -4091,7 +4185,7 @@
       <c r="D39">
         <v>0.77600000000000002</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E39" s="19">
         <v>0.86399999999999999</v>
       </c>
       <c r="H39" s="1"/>
@@ -4101,7 +4195,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="7">
         <v>2018</v>
       </c>
@@ -4114,7 +4208,7 @@
       <c r="D40" s="1">
         <v>0.80800000000000005</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="20">
         <v>0.96799999999999997</v>
       </c>
       <c r="F40" s="1"/>
@@ -4126,7 +4220,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
         <v>2019</v>
       </c>
@@ -4139,7 +4233,7 @@
       <c r="D41" s="1">
         <v>0.81599999999999995</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E41" s="20">
         <v>0.95599999999999996</v>
       </c>
       <c r="F41" s="1"/>
@@ -4151,7 +4245,7 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
         <v>2020</v>
       </c>
@@ -4164,7 +4258,7 @@
       <c r="D42" s="1">
         <v>0.84</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E42" s="20">
         <v>0.83499999999999996</v>
       </c>
       <c r="F42" s="1"/>
@@ -4176,7 +4270,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
         <v>2021</v>
       </c>
@@ -4189,13 +4283,13 @@
       <c r="D43" s="1">
         <v>0.875</v>
       </c>
-      <c r="E43" s="22">
+      <c r="E43" s="20">
         <v>0.872</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>2022</v>
       </c>
@@ -4208,10 +4302,10 @@
       <c r="D44" s="1">
         <v>0.84899999999999998</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="20">
         <v>0.93300000000000005</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F44" s="47" t="s">
         <v>33</v>
       </c>
       <c r="G44" s="1"/>
@@ -4222,7 +4316,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>2023</v>
       </c>
@@ -4235,10 +4329,10 @@
       <c r="D45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F45" s="35"/>
+      <c r="F45" s="48"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -4248,104 +4342,104 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:14" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27" t="s">
+    <row r="46" spans="1:14" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="26"/>
-    </row>
-    <row r="47" spans="1:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="14" t="s">
+      <c r="F46" s="58"/>
+    </row>
+    <row r="47" spans="1:14" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="21"/>
+      <c r="B47" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="57" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="36" t="s">
+    <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B52" s="37" t="s">
+      <c r="B52" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="38" t="s">
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G52" s="40" t="s">
+      <c r="G52" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="41" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="42">
+      <c r="B53" s="34">
         <v>1.24</v>
       </c>
-      <c r="C53" s="43" t="s">
+      <c r="C53" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="43" t="s">
+      <c r="D53" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="43" t="s">
+      <c r="E53" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F53" s="43" t="s">
+      <c r="F53" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G53" s="44" t="s">
+      <c r="G53" s="36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="45" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B54">
         <v>0.48</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="46" t="s">
+      <c r="D54" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="46" t="s">
+      <c r="E54" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="F54" s="46" t="s">
+      <c r="F54" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G54" s="47" t="s">
+      <c r="G54" s="39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="45" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B55">
@@ -4354,21 +4448,21 @@
       <c r="C55">
         <v>1.3149999999999999</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G55" s="48" t="s">
+      <c r="G55" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="45" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B56">
@@ -4377,21 +4471,21 @@
       <c r="C56">
         <v>1.6160000000000001</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G56" s="48" t="s">
+      <c r="G56" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="45" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B57">
@@ -4400,21 +4494,21 @@
       <c r="C57">
         <v>1.829</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G57" s="48" t="s">
+      <c r="G57" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="45" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B58">
@@ -4423,21 +4517,21 @@
       <c r="C58">
         <v>1.9470000000000001</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="48" t="s">
+      <c r="G58" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="45" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="37" t="s">
         <v>10</v>
       </c>
       <c r="B59">
@@ -4446,21 +4540,21 @@
       <c r="C59">
         <v>2.2509999999999999</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="48" t="s">
+      <c r="G59" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="45" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="37" t="s">
         <v>11</v>
       </c>
       <c r="B60">
@@ -4478,12 +4572,12 @@
       <c r="F60">
         <v>0.89300000000000002</v>
       </c>
-      <c r="G60" s="48">
+      <c r="G60" s="40">
         <v>2.42</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="45" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B61">
@@ -4501,12 +4595,12 @@
       <c r="F61">
         <v>1.06</v>
       </c>
-      <c r="G61" s="48">
+      <c r="G61" s="40">
         <v>3.3250000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="45" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B62">
@@ -4524,30 +4618,30 @@
       <c r="F62">
         <v>1.0409999999999999</v>
       </c>
-      <c r="G62" s="48">
+      <c r="G62" s="40">
         <v>3.6120000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="49" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B63" s="50" t="s">
+      <c r="B63" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="50" t="s">
+      <c r="C63" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="50" t="s">
+      <c r="D63" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E63" s="50" t="s">
+      <c r="E63" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="50" t="s">
+      <c r="F63" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="G63" s="51" t="s">
+      <c r="G63" s="43" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4563,11 +4657,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ca1cba85-b018-40b2-9d9a-243cd5b6fae5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4766,27 +4861,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ca1cba85-b018-40b2-9d9a-243cd5b6fae5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5E1B631-90B0-4D19-A35E-F8DC8BE167A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96E0334-A0AA-41B5-AE21-CAD1C9D10746}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f1fb8133-dfcb-4ab3-83e1-bcafde3f766a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ca1cba85-b018-40b2-9d9a-243cd5b6fae5"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4811,9 +4896,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96E0334-A0AA-41B5-AE21-CAD1C9D10746}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5E1B631-90B0-4D19-A35E-F8DC8BE167A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f1fb8133-dfcb-4ab3-83e1-bcafde3f766a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ca1cba85-b018-40b2-9d9a-243cd5b6fae5"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>